<commit_message>
validation added for the excel upload and downloadable template updated
</commit_message>
<xml_diff>
--- a/ntn_app/static/ntn_app/excel_template.xlsx
+++ b/ntn_app/static/ntn_app/excel_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rheann\Documents\CMU\Summer_24\Capstone\Central_DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMU_Capstone\ntn-backend\ntn_app\static\ntn_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B8B1A9-3D86-4F70-A273-EE307134ACAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF61A277-08E8-4C4D-8E92-1AC8AE9A0256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7D4E0957-2771-4500-BCDA-69AC7398D444}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>2yearCollegeName</t>
   </si>
@@ -56,25 +56,10 @@
     <t>Credits</t>
   </si>
   <si>
-    <t>Aarhus University</t>
-  </si>
-  <si>
-    <t>Aarhus,</t>
-  </si>
-  <si>
-    <t>Abertay University</t>
-  </si>
-  <si>
-    <t>Dundee,</t>
-  </si>
-  <si>
-    <t>BIOL</t>
-  </si>
-  <si>
-    <t>PSYC</t>
-  </si>
-  <si>
-    <t>ECTS</t>
+    <t>4yearCollegeName</t>
+  </si>
+  <si>
+    <t>4yearCollegeLocation</t>
   </si>
 </sst>
 </file>
@@ -98,27 +83,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCAEDFB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF95DCF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -126,40 +99,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A520CB89-20BD-4E2C-99BE-167EE2DD8007}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,9 +461,11 @@
     <col min="4" max="4" width="24.77734375" customWidth="1"/>
     <col min="5" max="5" width="30.77734375" customWidth="1"/>
     <col min="6" max="6" width="31.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,127 +484,62 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4">
-        <v>201608</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5">
-        <v>201608</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4">
-        <v>201608</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5">
-        <v>201608</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4">
-        <v>201608</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5">
-        <v>201608</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="5">
-        <v>2</v>
-      </c>
-    </row>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>